<commit_message>
encoder debug codes and speed control tune data
</commit_message>
<xml_diff>
--- a/results/gear_ratio/00_rpm-rads-converter.xlsx
+++ b/results/gear_ratio/00_rpm-rads-converter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all my files\documents\uvm\5_masters\hive\github_directory\results\gear_ratio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720EE667-C0A4-450A-AD8D-F4736B2EC8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEBE199-B471-4252-8536-D82D96159702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{042D6F52-7F9D-41D8-8769-957EA929A0A9}"/>
+    <workbookView xWindow="4710" yWindow="16200" windowWidth="14400" windowHeight="15600" xr2:uid="{042D6F52-7F9D-41D8-8769-957EA929A0A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>RPM &lt;&gt; rad/s converter</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>rad/s</t>
+  </si>
+  <si>
+    <t>&lt;</t>
   </si>
 </sst>
 </file>
@@ -416,20 +419,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0324E09-8731-4A66-B35D-E418AFB00C0D}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -437,16 +440,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <f>A4/9.549</f>
-        <v>17.384019269033409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12.566760917373548</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f>12/5.6</f>
+        <v>2.1428571428571428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -454,13 +466,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
       <c r="B7">
         <f>A7*9.549</f>
         <v>95.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>57/65</f>
+        <v>0.87692307692307692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>